<commit_message>
Sprint 2 updated backlog, week 1 burndown
</commit_message>
<xml_diff>
--- a/bookkeeping/sprint2/overview/s2_burndown.xlsx
+++ b/bookkeeping/sprint2/overview/s2_burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amee\Desktop\sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amee\git\ecse428group\bookkeeping\sprint2\overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -306,18 +303,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$D$4</c:f>
+              <c:f>Sheet1!$B$4:$I$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65</c:v>
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -423,67 +435,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61.904761904761905</c:v>
+                  <c:v>107.61904761904762</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58.80952380952381</c:v>
+                  <c:v>102.23809523809524</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55.714285714285715</c:v>
+                  <c:v>96.857142857142861</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.61904761904762</c:v>
+                  <c:v>91.476190476190482</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.523809523809526</c:v>
+                  <c:v>86.095238095238102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46.428571428571431</c:v>
+                  <c:v>80.714285714285722</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43.333333333333329</c:v>
+                  <c:v>75.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40.238095238095241</c:v>
+                  <c:v>69.952380952380949</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.142857142857139</c:v>
+                  <c:v>64.571428571428569</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.047619047619051</c:v>
+                  <c:v>59.19047619047619</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.952380952380949</c:v>
+                  <c:v>53.80952380952381</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.857142857142854</c:v>
+                  <c:v>48.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.761904761904759</c:v>
+                  <c:v>43.047619047619051</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.666666666666664</c:v>
+                  <c:v>37.666666666666671</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.571428571428569</c:v>
+                  <c:v>32.285714285714292</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.476190476190474</c:v>
+                  <c:v>26.904761904761898</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12.38095238095238</c:v>
+                  <c:v>21.523809523809518</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.2857142857142847</c:v>
+                  <c:v>16.142857142857139</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.1904761904761898</c:v>
+                  <c:v>10.761904761904759</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.0952380952380949</c:v>
+                  <c:v>5.3809523809523796</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0</c:v>
@@ -502,11 +514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-35570960"/>
-        <c:axId val="-35581840"/>
+        <c:axId val="-684460000"/>
+        <c:axId val="-684460544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-35570960"/>
+        <c:axId val="-684460000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42065"/>
@@ -542,14 +554,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35581840"/>
+        <c:crossAx val="-684460544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-35581840"/>
+        <c:axId val="-684460544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,7 +591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-35570960"/>
+        <c:crossAx val="-684460000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -636,88 +648,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="B2">
-            <v>42023</v>
-          </cell>
-          <cell r="C2">
-            <v>42024</v>
-          </cell>
-          <cell r="D2">
-            <v>42025</v>
-          </cell>
-          <cell r="E2">
-            <v>42026</v>
-          </cell>
-          <cell r="F2">
-            <v>42027</v>
-          </cell>
-          <cell r="G2">
-            <v>42028</v>
-          </cell>
-          <cell r="H2">
-            <v>42029</v>
-          </cell>
-          <cell r="I2">
-            <v>42030</v>
-          </cell>
-          <cell r="J2">
-            <v>42031</v>
-          </cell>
-          <cell r="K2">
-            <v>42032</v>
-          </cell>
-          <cell r="L2">
-            <v>42033</v>
-          </cell>
-          <cell r="M2">
-            <v>42034</v>
-          </cell>
-          <cell r="N2">
-            <v>42035</v>
-          </cell>
-          <cell r="O2">
-            <v>42036</v>
-          </cell>
-          <cell r="P2">
-            <v>42037</v>
-          </cell>
-          <cell r="Q2">
-            <v>42038</v>
-          </cell>
-          <cell r="R2">
-            <v>42039</v>
-          </cell>
-          <cell r="S2">
-            <v>42040</v>
-          </cell>
-          <cell r="T2">
-            <v>42041</v>
-          </cell>
-          <cell r="U2">
-            <v>42042</v>
-          </cell>
-          <cell r="V2">
-            <v>42043</v>
-          </cell>
-          <cell r="W2">
-            <v>42044</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -986,7 +916,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,87 +1003,87 @@
       </c>
       <c r="B3" s="2">
         <f>B20</f>
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C3" s="2">
         <f>B3-(B20/21)</f>
-        <v>61.904761904761905</v>
+        <v>107.61904761904762</v>
       </c>
       <c r="D3" s="2">
         <f>B3-(B3*2/21)</f>
-        <v>58.80952380952381</v>
+        <v>102.23809523809524</v>
       </c>
       <c r="E3" s="2">
         <f>B3-(B3*3/21)</f>
-        <v>55.714285714285715</v>
+        <v>96.857142857142861</v>
       </c>
       <c r="F3" s="2">
         <f>B3-(B3*4/21)</f>
-        <v>52.61904761904762</v>
+        <v>91.476190476190482</v>
       </c>
       <c r="G3" s="2">
         <f>B3-(B3*5/21)</f>
-        <v>49.523809523809526</v>
+        <v>86.095238095238102</v>
       </c>
       <c r="H3" s="2">
         <f>B3-(B3*6/21)</f>
-        <v>46.428571428571431</v>
+        <v>80.714285714285722</v>
       </c>
       <c r="I3" s="2">
         <f>B3-(B3*7/21)</f>
-        <v>43.333333333333329</v>
+        <v>75.333333333333343</v>
       </c>
       <c r="J3" s="2">
         <f>B3-(B3*8/21)</f>
-        <v>40.238095238095241</v>
+        <v>69.952380952380949</v>
       </c>
       <c r="K3" s="2">
         <f>B3-(B3*9/21)</f>
-        <v>37.142857142857139</v>
+        <v>64.571428571428569</v>
       </c>
       <c r="L3" s="2">
         <f>B3-(B3*10/21)</f>
-        <v>34.047619047619051</v>
+        <v>59.19047619047619</v>
       </c>
       <c r="M3" s="2">
         <f>B3-(B3*11/21)</f>
-        <v>30.952380952380949</v>
+        <v>53.80952380952381</v>
       </c>
       <c r="N3" s="2">
         <f>B3-(B3*12/21)</f>
-        <v>27.857142857142854</v>
+        <v>48.428571428571431</v>
       </c>
       <c r="O3" s="2">
         <f>B3-(B3*13/21)</f>
-        <v>24.761904761904759</v>
+        <v>43.047619047619051</v>
       </c>
       <c r="P3" s="2">
         <f>B3-(B3*14/21)</f>
-        <v>21.666666666666664</v>
+        <v>37.666666666666671</v>
       </c>
       <c r="Q3" s="2">
         <f>B3-(B3*15/21)</f>
-        <v>18.571428571428569</v>
+        <v>32.285714285714292</v>
       </c>
       <c r="R3" s="2">
         <f>B3-(B3*16/21)</f>
-        <v>15.476190476190474</v>
+        <v>26.904761904761898</v>
       </c>
       <c r="S3" s="2">
         <f>B3-(B3*17/21)</f>
-        <v>12.38095238095238</v>
+        <v>21.523809523809518</v>
       </c>
       <c r="T3" s="2">
         <f>B3-(B3*18/21)</f>
-        <v>9.2857142857142847</v>
+        <v>16.142857142857139</v>
       </c>
       <c r="U3" s="2">
         <f>B3-(B3*19/21)</f>
-        <v>6.1904761904761898</v>
+        <v>10.761904761904759</v>
       </c>
       <c r="V3" s="2">
         <f>B3-(B3*20/21)</f>
-        <v>3.0952380952380949</v>
+        <v>5.3809523809523796</v>
       </c>
       <c r="W3" s="2">
         <f>B3-(B3*21/21)</f>
@@ -1166,91 +1096,91 @@
       </c>
       <c r="B4">
         <f>B20</f>
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C4">
         <f>B4-B6</f>
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D4">
         <f>C4-C6</f>
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:W4" si="0">D4-D6</f>
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="V4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="W4">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -1264,19 +1194,19 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1358,7 +1288,7 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1368,7 +1298,7 @@
       </c>
       <c r="F11">
         <f>C11+D11+E11</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>19</v>
@@ -1426,10 +1356,10 @@
         <v>11</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1439,7 +1369,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1447,7 +1377,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1492,7 +1422,7 @@
         <v>11</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1502,7 +1432,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1510,10 +1440,10 @@
         <v>15</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1523,7 +1453,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,7 +1461,7 @@
         <v>16</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1553,11 +1483,11 @@
       </c>
       <c r="B20">
         <f>B11+B12+B13+B14+B15+B16+B17+B18+B19</f>
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="C20">
         <f>C11+C12+C13+C14+C15+C16+C17+C18+C19</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D20">
         <f>D11+D12+D13+D14+D15+D16+D17+D18+D19</f>
@@ -1569,7 +1499,7 @@
       </c>
       <c r="F20">
         <f>F11+F12+F13+F14+F15+F16+F17+F18+F19</f>
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>